<commit_message>
Develop tests and prepare results
</commit_message>
<xml_diff>
--- a/test_results/text_recognition.xlsx
+++ b/test_results/text_recognition.xlsx
@@ -8,30 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukaszkaminski/Studies/diploma/test_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD0A7A7-A802-B142-87DC-899C551C3254}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95C31AE-B457-3546-B0CF-BC228302597E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">test_results!$D$2:$D$250</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">test_results!$D$2:$D$250</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">test_results!$N$4</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">test_results!$D$2:$D$250</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">test_results!$D$2:$D$250</definedName>
+  </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="662">
   <si>
     <t>name</t>
   </si>
@@ -2017,48 +2013,6 @@
   </si>
   <si>
     <t>ENGIN E ERING SCIENCE -AND EDUCATION JoURNAL</t>
-  </si>
-  <si>
-    <t>range</t>
-  </si>
-  <si>
-    <t>count</t>
-  </si>
-  <si>
-    <t>(0.1; 0.2&gt;</t>
-  </si>
-  <si>
-    <t>(0.2; 0.3&gt;</t>
-  </si>
-  <si>
-    <t>(0.3; 0.4&gt;</t>
-  </si>
-  <si>
-    <t>(0.4; 0.5&gt;</t>
-  </si>
-  <si>
-    <t>(0.5; 0.6&gt;</t>
-  </si>
-  <si>
-    <t>(0.6; 0.7&gt;</t>
-  </si>
-  <si>
-    <t>(0.7; 0.8&gt;</t>
-  </si>
-  <si>
-    <t>(0.8; 0.9&gt;</t>
-  </si>
-  <si>
-    <t>(0.0; 0.1&gt;</t>
-  </si>
-  <si>
-    <t>0.0</t>
-  </si>
-  <si>
-    <t>(0.9; 1.0)</t>
-  </si>
-  <si>
-    <t>1.0</t>
   </si>
 </sst>
 </file>
@@ -2111,1199 +2065,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="pl-PL"/>
-              <a:t>Liczba przypadków testowych, których podobieństwo kosinusowe mieści się w określonym przedziale</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="9.7908468918600458E-2"/>
-          <c:y val="0.15194334767532777"/>
-          <c:w val="0.88185712189645515"/>
-          <c:h val="0.69646589203788234"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pl-PL"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>test_results!$F$2:$F$13</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>(0.0; 0.1&gt;</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>(0.1; 0.2&gt;</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>(0.2; 0.3&gt;</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>(0.3; 0.4&gt;</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>(0.4; 0.5&gt;</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>(0.5; 0.6&gt;</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>(0.6; 0.7&gt;</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>(0.7; 0.8&gt;</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>(0.8; 0.9&gt;</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>(0.9; 1.0)</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.0</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>test_results!$G$2:$G$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>76</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3AA8-1140-8B05-6E986C56AA4B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:dLblPos val="outEnd"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1225626704"/>
-        <c:axId val="1225655552"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1225626704"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="pl-PL"/>
-                  <a:t>Przedział wartości podobieństwa kosinusowego</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.35731591213950126"/>
-              <c:y val="0.92233013580596479"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pl-PL"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1225655552"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1225655552"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="pl-PL"/>
-                  <a:t>Liczba wystąpień wartości podobieśtwa kosizusowego</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="2.5752884417201943E-2"/>
-              <c:y val="0.18161652051375948"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pl-PL"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1225626704"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr>
-          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>4718</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>4427</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>670559</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>20320</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Wykres 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD81192D-CAC3-824D-896A-EC06C632AEB3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1991360</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>66040</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="65" cy="172227"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="pole tekstowe 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F79B2D9-576A-0349-9ED5-C76872517449}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11186160" y="2382520"/>
-          <a:ext cx="65" cy="172227"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="pl-PL" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3603,23 +2364,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G250"/>
+  <dimension ref="A1:D250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="125" zoomScaleNormal="258" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="58.6640625" customWidth="1"/>
-    <col min="2" max="2" width="62" customWidth="1"/>
-    <col min="3" max="3" width="43.83203125" customWidth="1"/>
-    <col min="4" max="4" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="19.83203125" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3632,14 +2390,8 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>662</v>
-      </c>
-      <c r="G1" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3652,15 +2404,8 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
-        <v>673</v>
-      </c>
-      <c r="G2">
-        <f>COUNTIFS(D2:D250, 0)</f>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3673,15 +2418,8 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>672</v>
-      </c>
-      <c r="G3">
-        <f>COUNTIFS(D2:D250, "&gt;0", D2:D250, "&lt;=0,1")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3694,15 +2432,8 @@
       <c r="D4">
         <v>0.99999999999999978</v>
       </c>
-      <c r="F4" t="s">
-        <v>664</v>
-      </c>
-      <c r="G4">
-        <f>COUNTIFS(D2:D250, "&gt;0,1", D2:D250, "&lt;=0,2")</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -3713,17 +2444,10 @@
         <v>15</v>
       </c>
       <c r="D5">
-        <v>1.0000000000000002</v>
-      </c>
-      <c r="F5" t="s">
-        <v>665</v>
-      </c>
-      <c r="G5">
-        <f>COUNTIFS(D2:D250, "&gt;0,2", D2:D250, "&lt;=0,3")</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -3736,15 +2460,8 @@
       <c r="D6">
         <v>0.53452248382484868</v>
       </c>
-      <c r="F6" t="s">
-        <v>666</v>
-      </c>
-      <c r="G6">
-        <f>COUNTIFS(D2:D250, "&gt;0,3", D2:D250, "&lt;=0,4")</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -3757,15 +2474,8 @@
       <c r="D7">
         <v>0.70710678118654746</v>
       </c>
-      <c r="F7" t="s">
-        <v>667</v>
-      </c>
-      <c r="G7">
-        <f>COUNTIFS(D2:D250, "&gt;0,4", D2:D250, "&lt;=0,5")</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -3778,15 +2488,8 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="F8" t="s">
-        <v>668</v>
-      </c>
-      <c r="G8">
-        <f>COUNTIFS(D2:D250, "&gt;0,5", D2:D250, "&lt;=0,6")</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -3799,15 +2502,8 @@
       <c r="D9">
         <v>0.99999999999999978</v>
       </c>
-      <c r="F9" t="s">
-        <v>669</v>
-      </c>
-      <c r="G9">
-        <f>COUNTIFS(D2:D250, "&gt;0,6", D2:D250, "&lt;=0,7")</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -3820,15 +2516,8 @@
       <c r="D10">
         <v>0.79999999999999982</v>
       </c>
-      <c r="F10" t="s">
-        <v>670</v>
-      </c>
-      <c r="G10">
-        <f>COUNTIFS(D2:D250, "&gt;0,7", D2:D250, "&lt;=0,8")</f>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -3839,17 +2528,10 @@
         <v>31</v>
       </c>
       <c r="D11">
-        <v>1.0000000000000002</v>
-      </c>
-      <c r="F11" t="s">
-        <v>671</v>
-      </c>
-      <c r="G11">
-        <f>COUNTIFS(D2:D250, "&gt;0,8", D2:D250, "&lt;=0,9")</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -3862,15 +2544,8 @@
       <c r="D12">
         <v>0.20412414523193154</v>
       </c>
-      <c r="F12" t="s">
-        <v>674</v>
-      </c>
-      <c r="G12">
-        <f>COUNTIFS(D2:D250, "&gt;0,9", D2:D250, "&lt;1")</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -3883,15 +2558,8 @@
       <c r="D13">
         <v>0.6761234037828131</v>
       </c>
-      <c r="F13" t="s">
-        <v>675</v>
-      </c>
-      <c r="G13">
-        <f>COUNTIFS(D2:D250, 1)</f>
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -3905,7 +2573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -3919,7 +2587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -4378,7 +3046,7 @@
         <v>134</v>
       </c>
       <c r="D48">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -4574,7 +3242,7 @@
         <v>176</v>
       </c>
       <c r="D62">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -4630,7 +3298,7 @@
         <v>188</v>
       </c>
       <c r="D66">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -4644,7 +3312,7 @@
         <v>191</v>
       </c>
       <c r="D67">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -4714,7 +3382,7 @@
         <v>206</v>
       </c>
       <c r="D72">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -4854,7 +3522,7 @@
         <v>235</v>
       </c>
       <c r="D82">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -4952,7 +3620,7 @@
         <v>255</v>
       </c>
       <c r="D89">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -5120,7 +3788,7 @@
         <v>288</v>
       </c>
       <c r="D101">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -5288,7 +3956,7 @@
         <v>319</v>
       </c>
       <c r="D113">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -5428,7 +4096,7 @@
         <v>347</v>
       </c>
       <c r="D123">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
@@ -5610,7 +4278,7 @@
         <v>378</v>
       </c>
       <c r="D136">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
@@ -5820,7 +4488,7 @@
         <v>418</v>
       </c>
       <c r="D151">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
@@ -6408,7 +5076,7 @@
         <v>528</v>
       </c>
       <c r="D193">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
@@ -6520,7 +5188,7 @@
         <v>546</v>
       </c>
       <c r="D201">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
@@ -6604,7 +5272,7 @@
         <v>560</v>
       </c>
       <c r="D207">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
@@ -6660,7 +5328,7 @@
         <v>571</v>
       </c>
       <c r="D211">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
@@ -6800,7 +5468,7 @@
         <v>597</v>
       </c>
       <c r="D221">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
@@ -7080,7 +5748,7 @@
         <v>235</v>
       </c>
       <c r="D241">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
@@ -7178,7 +5846,7 @@
         <v>657</v>
       </c>
       <c r="D248">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
@@ -7192,7 +5860,7 @@
         <v>657</v>
       </c>
       <c r="D249">
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
@@ -7211,6 +5879,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Develop plots in Excel files
</commit_message>
<xml_diff>
--- a/test_results/text_recognition.xlsx
+++ b/test_results/text_recognition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukaszkaminski/Studies/diploma/test_results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumenty\Sem. 7 2020Z\Praca dyplomowa\diploma\test_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95C31AE-B457-3546-B0CF-BC228302597E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671806D0-FD51-4E4A-A26D-6F6A862852CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_results" sheetId="1" r:id="rId1"/>
@@ -18,16 +18,23 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">test_results!$D$2:$D$250</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">test_results!$D$2:$D$250</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">test_results!$N$4</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">test_results!$D$2:$D$250</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">test_results!$D$2:$D$250</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="665">
   <si>
     <t>name</t>
   </si>
@@ -2013,6 +2020,15 @@
   </si>
   <si>
     <t>ENGIN E ERING SCIENCE -AND EDUCATION JoURNAL</t>
+  </si>
+  <si>
+    <t>cosine_similarity_max_count</t>
+  </si>
+  <si>
+    <t>cosine_similarity_min_count</t>
+  </si>
+  <si>
+    <t>cosine_similarity_average</t>
   </si>
 </sst>
 </file>
@@ -2065,6 +2081,773 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.0</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Histogram wartości podobieństwa kosinusowego</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Histogram wartości podobieństwa kosinusowego</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{B8B41EF2-B268-4608-9816-4DA016BD6DF2}">
+          <cx:dataLabels pos="outEnd">
+            <cx:txPr>
+              <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" rtl="0">
+                  <a:defRPr sz="900" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL">
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </cx:txPr>
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r">
+              <cx:binSize val="0.10000000000000001"/>
+            </cx:binning>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0.100000001"/>
+        <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="900" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="900" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+  <cx:printSettings>
+    <cx:headerFooter alignWithMargins="1" differentOddEven="0" differentFirst="0"/>
+    <cx:pageMargins l="0.69999999999999996" r="0.69999999999999996" t="0.75" b="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+    <cx:pageSetup paperSize="1" firstPageNumber="1" orientation="default" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  </cx:printSettings>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>601662</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>179068</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>341862</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>121468</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Wykres 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E606CB9-71BE-4765-A696-EAB76C8189B1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10210482" y="179068"/>
+              <a:ext cx="5760000" cy="3600000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100"/>
+                <a:t>Ten wykres jest niedostępny w Twojej wersji programu Excel.
+Edytowanie tego kształtu lub zapisanie tego skoroszytu w innym formacie pliku spowoduje trwałe uszkodzenie wykresu.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2364,20 +3147,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D250"/>
+  <dimension ref="A1:Q250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="1" max="1" width="60.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
     <col min="3" max="3" width="35.33203125" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" customWidth="1"/>
+    <col min="13" max="13" width="8.77734375" customWidth="1"/>
+    <col min="16" max="16" width="25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2391,7 +3179,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2404,8 +3192,15 @@
       <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="P2" t="s">
+        <v>663</v>
+      </c>
+      <c r="Q2">
+        <f>COUNTIF(D2:D250, 0)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2418,8 +3213,15 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="P3" t="s">
+        <v>662</v>
+      </c>
+      <c r="Q3">
+        <f>COUNTIF(D2:D250, 1)</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2432,8 +3234,15 @@
       <c r="D4">
         <v>0.99999999999999978</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="P4" t="s">
+        <v>664</v>
+      </c>
+      <c r="Q4">
+        <f>AVERAGE(D2:D250)</f>
+        <v>0.64243973829343293</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -2447,7 +3256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2461,7 +3270,7 @@
         <v>0.53452248382484868</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2475,7 +3284,7 @@
         <v>0.70710678118654746</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2489,7 +3298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -2503,7 +3312,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -2517,7 +3326,7 @@
         <v>0.79999999999999982</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2531,7 +3340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -2545,7 +3354,7 @@
         <v>0.20412414523193154</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -2559,7 +3368,7 @@
         <v>0.6761234037828131</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -2573,7 +3382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -2587,7 +3396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -2601,7 +3410,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -2615,7 +3424,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -2629,7 +3438,7 @@
         <v>0.50709255283710986</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -2643,7 +3452,7 @@
         <v>0.57735026918962584</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -2657,7 +3466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -2671,7 +3480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -2685,7 +3494,7 @@
         <v>0.86602540378443871</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -2699,7 +3508,7 @@
         <v>0.63900965042269375</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -2713,7 +3522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -2727,7 +3536,7 @@
         <v>0.67082039324993692</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -2741,7 +3550,7 @@
         <v>0.61237243569579458</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>74</v>
       </c>
@@ -2755,7 +3564,7 @@
         <v>0.904534033733291</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>77</v>
       </c>
@@ -2769,7 +3578,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>80</v>
       </c>
@@ -2783,7 +3592,7 @@
         <v>0.89973541084243736</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>83</v>
       </c>
@@ -2797,7 +3606,7 @@
         <v>0.89442719099991586</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -2811,7 +3620,7 @@
         <v>0.70710678118654746</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -2825,7 +3634,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>91</v>
       </c>
@@ -2839,7 +3648,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>93</v>
       </c>
@@ -2853,7 +3662,7 @@
         <v>0.40824829046386296</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>96</v>
       </c>
@@ -2867,7 +3676,7 @@
         <v>0.74999999999999989</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>99</v>
       </c>
@@ -2881,7 +3690,7 @@
         <v>0.84615384615384626</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>102</v>
       </c>
@@ -2895,7 +3704,7 @@
         <v>0.47809144373375745</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>105</v>
       </c>
@@ -2909,7 +3718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>108</v>
       </c>
@@ -2923,7 +3732,7 @@
         <v>0.86602540378443871</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>111</v>
       </c>
@@ -2937,7 +3746,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>113</v>
       </c>
@@ -2951,7 +3760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>116</v>
       </c>
@@ -2965,7 +3774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>119</v>
       </c>
@@ -2979,7 +3788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>122</v>
       </c>
@@ -2993,7 +3802,7 @@
         <v>0.66815310478106094</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>125</v>
       </c>
@@ -3007,7 +3816,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>128</v>
       </c>
@@ -3021,7 +3830,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>130</v>
       </c>
@@ -3035,7 +3844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>133</v>
       </c>
@@ -3049,7 +3858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>135</v>
       </c>
@@ -3063,7 +3872,7 @@
         <v>0.7745966692414834</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>138</v>
       </c>
@@ -3077,7 +3886,7 @@
         <v>0.78262379212492639</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>141</v>
       </c>
@@ -3091,7 +3900,7 @@
         <v>0.57735026918962584</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>144</v>
       </c>
@@ -3105,7 +3914,7 @@
         <v>0.79999999999999982</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>147</v>
       </c>
@@ -3119,7 +3928,7 @@
         <v>0.83333333333333348</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>150</v>
       </c>
@@ -3133,7 +3942,7 @@
         <v>0.73029674334022143</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>153</v>
       </c>
@@ -3147,7 +3956,7 @@
         <v>0.43301270189221935</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>156</v>
       </c>
@@ -3161,7 +3970,7 @@
         <v>0.89442719099991586</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>159</v>
       </c>
@@ -3175,7 +3984,7 @@
         <v>0.77151674981045948</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>162</v>
       </c>
@@ -3189,7 +3998,7 @@
         <v>0.63245553203367588</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>165</v>
       </c>
@@ -3203,7 +4012,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>168</v>
       </c>
@@ -3217,7 +4026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>171</v>
       </c>
@@ -3231,7 +4040,7 @@
         <v>0.89442719099991586</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>174</v>
       </c>
@@ -3245,7 +4054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>177</v>
       </c>
@@ -3259,7 +4068,7 @@
         <v>0.20412414523193154</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>180</v>
       </c>
@@ -3273,7 +4082,7 @@
         <v>0.80403025220736968</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>183</v>
       </c>
@@ -3287,7 +4096,7 @@
         <v>0.78262379212492639</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>186</v>
       </c>
@@ -3301,7 +4110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>189</v>
       </c>
@@ -3315,7 +4124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>192</v>
       </c>
@@ -3329,7 +4138,7 @@
         <v>0.50709255283710986</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>195</v>
       </c>
@@ -3343,7 +4152,7 @@
         <v>0.9285714285714286</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>198</v>
       </c>
@@ -3357,7 +4166,7 @@
         <v>0.63960214906683133</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>201</v>
       </c>
@@ -3371,7 +4180,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>204</v>
       </c>
@@ -3385,7 +4194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>207</v>
       </c>
@@ -3399,7 +4208,7 @@
         <v>0.15430334996209191</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>210</v>
       </c>
@@ -3413,7 +4222,7 @@
         <v>0.36514837167011072</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>213</v>
       </c>
@@ -3427,7 +4236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>216</v>
       </c>
@@ -3441,7 +4250,7 @@
         <v>0.93541434669348522</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>219</v>
       </c>
@@ -3455,7 +4264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>222</v>
       </c>
@@ -3469,7 +4278,7 @@
         <v>0.27386127875258304</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>225</v>
       </c>
@@ -3483,7 +4292,7 @@
         <v>0.63960214906683133</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>228</v>
       </c>
@@ -3497,7 +4306,7 @@
         <v>0.70710678118654746</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>231</v>
       </c>
@@ -3511,7 +4320,7 @@
         <v>0.77611400011626552</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>234</v>
       </c>
@@ -3525,7 +4334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>236</v>
       </c>
@@ -3539,7 +4348,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>239</v>
       </c>
@@ -3553,7 +4362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>242</v>
       </c>
@@ -3567,7 +4376,7 @@
         <v>0.57735026918962584</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>245</v>
       </c>
@@ -3581,7 +4390,7 @@
         <v>0.57735026918962584</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>248</v>
       </c>
@@ -3595,7 +4404,7 @@
         <v>0.57735026918962584</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>251</v>
       </c>
@@ -3609,7 +4418,7 @@
         <v>0.7453559924999299</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>254</v>
       </c>
@@ -3623,7 +4432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>256</v>
       </c>
@@ -3637,7 +4446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>259</v>
       </c>
@@ -3651,7 +4460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>261</v>
       </c>
@@ -3665,7 +4474,7 @@
         <v>0.76271276980969005</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>264</v>
       </c>
@@ -3679,7 +4488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>267</v>
       </c>
@@ -3693,7 +4502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>269</v>
       </c>
@@ -3707,7 +4516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>271</v>
       </c>
@@ -3721,7 +4530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>274</v>
       </c>
@@ -3735,7 +4544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>277</v>
       </c>
@@ -3749,7 +4558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>280</v>
       </c>
@@ -3763,7 +4572,7 @@
         <v>0.39999999999999991</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>283</v>
       </c>
@@ -3777,7 +4586,7 @@
         <v>0.79999999999999982</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>286</v>
       </c>
@@ -3791,7 +4600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>289</v>
       </c>
@@ -3805,7 +4614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>291</v>
       </c>
@@ -3819,7 +4628,7 @@
         <v>0.28867513459481292</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>294</v>
       </c>
@@ -3833,7 +4642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>296</v>
       </c>
@@ -3847,7 +4656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>298</v>
       </c>
@@ -3861,7 +4670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>300</v>
       </c>
@@ -3875,7 +4684,7 @@
         <v>0.57735026918962584</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>303</v>
       </c>
@@ -3889,7 +4698,7 @@
         <v>0.70710678118654757</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>306</v>
       </c>
@@ -3903,7 +4712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>309</v>
       </c>
@@ -3917,7 +4726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>312</v>
       </c>
@@ -3931,7 +4740,7 @@
         <v>0.33806170189140655</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>315</v>
       </c>
@@ -3945,7 +4754,7 @@
         <v>0.44721359549995793</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>318</v>
       </c>
@@ -3959,7 +4768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>320</v>
       </c>
@@ -3973,7 +4782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>323</v>
       </c>
@@ -3987,7 +4796,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>326</v>
       </c>
@@ -4001,7 +4810,7 @@
         <v>0.59999999999999987</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>329</v>
       </c>
@@ -4015,7 +4824,7 @@
         <v>0.7559289460184544</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>332</v>
       </c>
@@ -4029,7 +4838,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>335</v>
       </c>
@@ -4043,7 +4852,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>337</v>
       </c>
@@ -4057,7 +4866,7 @@
         <v>0.54433105395181736</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>340</v>
       </c>
@@ -4071,7 +4880,7 @@
         <v>0.35355339059327373</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>343</v>
       </c>
@@ -4085,7 +4894,7 @@
         <v>0.54772255750516607</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>346</v>
       </c>
@@ -4099,7 +4908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>348</v>
       </c>
@@ -4113,7 +4922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>350</v>
       </c>
@@ -4127,7 +4936,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>352</v>
       </c>
@@ -4141,7 +4950,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>354</v>
       </c>
@@ -4155,7 +4964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>356</v>
       </c>
@@ -4169,7 +4978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>358</v>
       </c>
@@ -4183,7 +4992,7 @@
         <v>0.7627700713964739</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>361</v>
       </c>
@@ -4197,7 +5006,7 @@
         <v>0.8999999999999998</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>364</v>
       </c>
@@ -4211,7 +5020,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>366</v>
       </c>
@@ -4225,7 +5034,7 @@
         <v>0.94491118252306805</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>369</v>
       </c>
@@ -4239,7 +5048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>371</v>
       </c>
@@ -4253,7 +5062,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>374</v>
       </c>
@@ -4267,7 +5076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>377</v>
       </c>
@@ -4281,7 +5090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>379</v>
       </c>
@@ -4295,7 +5104,7 @@
         <v>0.92307692307692324</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>382</v>
       </c>
@@ -4309,7 +5118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>385</v>
       </c>
@@ -4323,7 +5132,7 @@
         <v>0.5163977794943222</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>388</v>
       </c>
@@ -4337,7 +5146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>390</v>
       </c>
@@ -4351,7 +5160,7 @@
         <v>0.7627700713964739</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>393</v>
       </c>
@@ -4365,7 +5174,7 @@
         <v>0.70710678118654746</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>396</v>
       </c>
@@ -4379,7 +5188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>399</v>
       </c>
@@ -4393,7 +5202,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>401</v>
       </c>
@@ -4407,7 +5216,7 @@
         <v>0.87499999999999978</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>404</v>
       </c>
@@ -4421,7 +5230,7 @@
         <v>0.83333333333333348</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>407</v>
       </c>
@@ -4435,7 +5244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>409</v>
       </c>
@@ -4449,7 +5258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>411</v>
       </c>
@@ -4463,7 +5272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>414</v>
       </c>
@@ -4477,7 +5286,7 @@
         <v>0.89442719099991586</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>417</v>
       </c>
@@ -4491,7 +5300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>419</v>
       </c>
@@ -4505,7 +5314,7 @@
         <v>0.86602540378443871</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>422</v>
       </c>
@@ -4519,7 +5328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>425</v>
       </c>
@@ -4533,7 +5342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>428</v>
       </c>
@@ -4547,7 +5356,7 @@
         <v>0.83333333333333348</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>431</v>
       </c>
@@ -4561,7 +5370,7 @@
         <v>0.2581988897471611</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>434</v>
       </c>
@@ -4575,7 +5384,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>437</v>
       </c>
@@ -4589,7 +5398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>438</v>
       </c>
@@ -4603,7 +5412,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>441</v>
       </c>
@@ -4617,7 +5426,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>444</v>
       </c>
@@ -4631,7 +5440,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>447</v>
       </c>
@@ -4645,7 +5454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>449</v>
       </c>
@@ -4659,7 +5468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>451</v>
       </c>
@@ -4673,7 +5482,7 @@
         <v>0.59999999999999987</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>454</v>
       </c>
@@ -4687,7 +5496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>457</v>
       </c>
@@ -4701,7 +5510,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>459</v>
       </c>
@@ -4715,7 +5524,7 @@
         <v>0.62897090203315098</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>462</v>
       </c>
@@ -4729,7 +5538,7 @@
         <v>0.70710678118654746</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>465</v>
       </c>
@@ -4743,7 +5552,7 @@
         <v>0.89442719099991586</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>468</v>
       </c>
@@ -4757,7 +5566,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>471</v>
       </c>
@@ -4771,7 +5580,7 @@
         <v>0.10050378152592121</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>474</v>
       </c>
@@ -4785,7 +5594,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>476</v>
       </c>
@@ -4799,7 +5608,7 @@
         <v>0.86602540378443871</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>479</v>
       </c>
@@ -4813,7 +5622,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>481</v>
       </c>
@@ -4827,7 +5636,7 @@
         <v>0.22360679774997896</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>484</v>
       </c>
@@ -4841,7 +5650,7 @@
         <v>0.92582009977255142</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>487</v>
       </c>
@@ -4855,7 +5664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>489</v>
       </c>
@@ -4869,7 +5678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>491</v>
       </c>
@@ -4883,7 +5692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>493</v>
       </c>
@@ -4897,7 +5706,7 @@
         <v>0.79999999999999982</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>494</v>
       </c>
@@ -4911,7 +5720,7 @@
         <v>0.54772255750516607</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>497</v>
       </c>
@@ -4925,7 +5734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>500</v>
       </c>
@@ -4939,7 +5748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>503</v>
       </c>
@@ -4953,7 +5762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>505</v>
       </c>
@@ -4967,7 +5776,7 @@
         <v>0.66815310478106094</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>508</v>
       </c>
@@ -4981,7 +5790,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>510</v>
       </c>
@@ -4995,7 +5804,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>513</v>
       </c>
@@ -5009,7 +5818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>516</v>
       </c>
@@ -5023,7 +5832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>519</v>
       </c>
@@ -5037,7 +5846,7 @@
         <v>0.40824829046386296</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>522</v>
       </c>
@@ -5051,7 +5860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>524</v>
       </c>
@@ -5065,7 +5874,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>527</v>
       </c>
@@ -5079,7 +5888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>529</v>
       </c>
@@ -5093,7 +5902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>531</v>
       </c>
@@ -5107,7 +5916,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>533</v>
       </c>
@@ -5121,7 +5930,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>535</v>
       </c>
@@ -5135,7 +5944,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>537</v>
       </c>
@@ -5149,7 +5958,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>539</v>
       </c>
@@ -5163,7 +5972,7 @@
         <v>0.40824829046386296</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>542</v>
       </c>
@@ -5177,7 +5986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>545</v>
       </c>
@@ -5191,7 +6000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>547</v>
       </c>
@@ -5205,7 +6014,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>550</v>
       </c>
@@ -5219,7 +6028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>552</v>
       </c>
@@ -5233,7 +6042,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>554</v>
       </c>
@@ -5247,7 +6056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>556</v>
       </c>
@@ -5261,7 +6070,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>559</v>
       </c>
@@ -5275,7 +6084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>561</v>
       </c>
@@ -5289,7 +6098,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>564</v>
       </c>
@@ -5303,7 +6112,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>567</v>
       </c>
@@ -5317,7 +6126,7 @@
         <v>0.50000000000000011</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>570</v>
       </c>
@@ -5331,7 +6140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>572</v>
       </c>
@@ -5345,7 +6154,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>575</v>
       </c>
@@ -5359,7 +6168,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>577</v>
       </c>
@@ -5373,7 +6182,7 @@
         <v>0.81649658092772592</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>580</v>
       </c>
@@ -5387,7 +6196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>583</v>
       </c>
@@ -5401,7 +6210,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>586</v>
       </c>
@@ -5415,7 +6224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>588</v>
       </c>
@@ -5429,7 +6238,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>590</v>
       </c>
@@ -5443,7 +6252,7 @@
         <v>0.7745966692414834</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>593</v>
       </c>
@@ -5457,7 +6266,7 @@
         <v>0.7745966692414834</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>596</v>
       </c>
@@ -5471,7 +6280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>598</v>
       </c>
@@ -5485,7 +6294,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>601</v>
       </c>
@@ -5499,7 +6308,7 @@
         <v>0.67082039324993692</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>604</v>
       </c>
@@ -5513,7 +6322,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>607</v>
       </c>
@@ -5527,7 +6336,7 @@
         <v>0.57735026918962584</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>610</v>
       </c>
@@ -5541,7 +6350,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>613</v>
       </c>
@@ -5555,7 +6364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>615</v>
       </c>
@@ -5569,7 +6378,7 @@
         <v>0.3779644730092272</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>618</v>
       </c>
@@ -5583,7 +6392,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>621</v>
       </c>
@@ -5597,7 +6406,7 @@
         <v>0.89442719099991586</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>624</v>
       </c>
@@ -5611,7 +6420,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>627</v>
       </c>
@@ -5625,7 +6434,7 @@
         <v>0.1889822365046136</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>629</v>
       </c>
@@ -5639,7 +6448,7 @@
         <v>0.18257418583505536</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>631</v>
       </c>
@@ -5653,7 +6462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>632</v>
       </c>
@@ -5667,7 +6476,7 @@
         <v>0.88191710368819687</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>634</v>
       </c>
@@ -5681,7 +6490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>635</v>
       </c>
@@ -5695,7 +6504,7 @@
         <v>0.40824829046386296</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>637</v>
       </c>
@@ -5709,7 +6518,7 @@
         <v>0.74999999999999989</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>639</v>
       </c>
@@ -5723,7 +6532,7 @@
         <v>0.70710678118654746</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>641</v>
       </c>
@@ -5737,7 +6546,7 @@
         <v>0.77611400011626552</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>643</v>
       </c>
@@ -5751,7 +6560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>644</v>
       </c>
@@ -5765,7 +6574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>645</v>
       </c>
@@ -5779,7 +6588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>646</v>
       </c>
@@ -5793,7 +6602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>647</v>
       </c>
@@ -5807,7 +6616,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>650</v>
       </c>
@@ -5821,7 +6630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>653</v>
       </c>
@@ -5835,7 +6644,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>656</v>
       </c>
@@ -5849,7 +6658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>658</v>
       </c>
@@ -5863,7 +6672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>659</v>
       </c>
@@ -5879,5 +6688,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>